<commit_message>
Remove duplicate in team results
</commit_message>
<xml_diff>
--- a/Results 2025 MASTER.xlsx
+++ b/Results 2025 MASTER.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sd44o365-my.sharepoint.com/personal/19247_sd44_ca/Documents/nsssaa-mtb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="741" documentId="8_{959BACE5-4009-4EA9-89AA-0ADE5BBDFC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA173E67-7C3E-47DD-A166-2F8EFE739D0B}"/>
+  <xr:revisionPtr revIDLastSave="745" documentId="8_{959BACE5-4009-4EA9-89AA-0ADE5BBDFC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98BE2E0B-65CF-4C7C-B57F-338F9F1DB728}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="-21600" windowWidth="19200" windowHeight="21020" firstSheet="5" activeTab="5" xr2:uid="{EF65BA04-60F3-4F2B-BC8E-976066A335E4}"/>
+    <workbookView xWindow="240" yWindow="-21540" windowWidth="23040" windowHeight="20400" tabRatio="669" activeTab="5" xr2:uid="{EF65BA04-60F3-4F2B-BC8E-976066A335E4}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER ROSTERS" sheetId="15" r:id="rId1"/>
     <sheet name="PTS" sheetId="3" state="hidden" r:id="rId2"/>
-    <sheet name="TeamHelper" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="TeamHelper" sheetId="5" r:id="rId3"/>
     <sheet name="Lists" sheetId="8" state="hidden" r:id="rId4"/>
     <sheet name="Individual Results" sheetId="2" r:id="rId5"/>
     <sheet name="TeamPoints" sheetId="11" r:id="rId6"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -17486,7 +17486,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EE6F0-5209-4548-B73C-37B54C96BA68}">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -40074,10 +40076,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C807E2-9D8B-4820-9B4A-3D4F64F10F5D}">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J88" sqref="J88"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -40211,7 +40213,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="129">
-        <f>SUM(C2:H2)</f>
+        <f t="shared" ref="I2:I33" si="0">SUM(C2:H2)</f>
         <v>225</v>
       </c>
     </row>
@@ -40309,7 +40311,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="129">
-        <f>SUM(C3:H3)</f>
+        <f t="shared" si="0"/>
         <v>220</v>
       </c>
     </row>
@@ -40407,7 +40409,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="129">
-        <f>SUM(C4:H4)</f>
+        <f t="shared" si="0"/>
         <v>183</v>
       </c>
     </row>
@@ -40505,7 +40507,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="129">
-        <f>SUM(C5:H5)</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
     </row>
@@ -40603,7 +40605,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="129">
-        <f>SUM(C6:H6)</f>
+        <f t="shared" si="0"/>
         <v>114</v>
       </c>
     </row>
@@ -40701,7 +40703,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="129">
-        <f>SUM(C7:H7)</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
     </row>
@@ -40799,7 +40801,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="129">
-        <f>SUM(C8:H8)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -40897,7 +40899,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="129">
-        <f>SUM(C9:H9)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
@@ -40995,7 +40997,7 @@
         <v/>
       </c>
       <c r="I10" s="129">
-        <f>SUM(C10:H10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41093,7 +41095,7 @@
         <v/>
       </c>
       <c r="I11" s="129">
-        <f>SUM(C11:H11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41191,7 +41193,7 @@
         <v/>
       </c>
       <c r="I12" s="129">
-        <f>SUM(C12:H12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41289,7 +41291,7 @@
         <v/>
       </c>
       <c r="I13" s="129">
-        <f>SUM(C13:H13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41387,7 +41389,7 @@
         <v/>
       </c>
       <c r="I14" s="129">
-        <f>SUM(C14:H14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41485,7 +41487,7 @@
         <v/>
       </c>
       <c r="I15" s="129">
-        <f>SUM(C15:H15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41583,7 +41585,7 @@
         <v/>
       </c>
       <c r="I16" s="129">
-        <f>SUM(C16:H16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41681,7 +41683,7 @@
         <v/>
       </c>
       <c r="I17" s="129">
-        <f>SUM(C17:H17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41779,7 +41781,7 @@
         <v/>
       </c>
       <c r="I18" s="129">
-        <f>SUM(C18:H18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41877,7 +41879,7 @@
         <v/>
       </c>
       <c r="I19" s="129">
-        <f>SUM(C19:H19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -41975,7 +41977,7 @@
         <v/>
       </c>
       <c r="I20" s="129">
-        <f>SUM(C20:H20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42073,7 +42075,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="130">
-        <f>SUM(C21:H21)</f>
+        <f t="shared" si="0"/>
         <v>250</v>
       </c>
     </row>
@@ -42171,7 +42173,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="130">
-        <f>SUM(C22:H22)</f>
+        <f t="shared" si="0"/>
         <v>245</v>
       </c>
     </row>
@@ -42269,7 +42271,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="130">
-        <f>SUM(C23:H23)</f>
+        <f t="shared" si="0"/>
         <v>245</v>
       </c>
     </row>
@@ -42367,7 +42369,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="130">
-        <f>SUM(C24:H24)</f>
+        <f t="shared" si="0"/>
         <v>190</v>
       </c>
     </row>
@@ -42465,7 +42467,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="130">
-        <f>SUM(C25:H25)</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
@@ -42563,7 +42565,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="130">
-        <f>SUM(C26:H26)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
@@ -42661,7 +42663,7 @@
         <v/>
       </c>
       <c r="I27" s="130">
-        <f>SUM(C27:H27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42759,7 +42761,7 @@
         <v/>
       </c>
       <c r="I28" s="130">
-        <f>SUM(C28:H28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42857,7 +42859,7 @@
         <v/>
       </c>
       <c r="I29" s="130">
-        <f>SUM(C29:H29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42955,7 +42957,7 @@
         <v/>
       </c>
       <c r="I30" s="130">
-        <f>SUM(C30:H30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43053,7 +43055,7 @@
         <v/>
       </c>
       <c r="I31" s="130">
-        <f>SUM(C31:H31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43151,7 +43153,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="131">
-        <f>SUM(C32:H32)</f>
+        <f t="shared" si="0"/>
         <v>275</v>
       </c>
     </row>
@@ -43249,7 +43251,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="131">
-        <f>SUM(C33:H33)</f>
+        <f t="shared" si="0"/>
         <v>164</v>
       </c>
     </row>
@@ -43347,7 +43349,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="131">
-        <f>SUM(C34:H34)</f>
+        <f t="shared" ref="I34:I65" si="1">SUM(C34:H34)</f>
         <v>158</v>
       </c>
     </row>
@@ -43445,7 +43447,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="131">
-        <f>SUM(C35:H35)</f>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
     </row>
@@ -43543,7 +43545,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="131">
-        <f>SUM(C36:H36)</f>
+        <f t="shared" si="1"/>
         <v>132</v>
       </c>
     </row>
@@ -43641,7 +43643,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="131">
-        <f>SUM(C37:H37)</f>
+        <f t="shared" si="1"/>
         <v>122</v>
       </c>
     </row>
@@ -43739,7 +43741,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="131">
-        <f>SUM(C38:H38)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
@@ -43837,7 +43839,7 @@
         <v/>
       </c>
       <c r="I39" s="131">
-        <f>SUM(C39:H39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -43935,7 +43937,7 @@
         <v/>
       </c>
       <c r="I40" s="131">
-        <f>SUM(C40:H40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44033,7 +44035,7 @@
         <v/>
       </c>
       <c r="I41" s="131">
-        <f>SUM(C41:H41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44131,7 +44133,7 @@
         <v/>
       </c>
       <c r="I42" s="131">
-        <f>SUM(C42:H42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44229,7 +44231,7 @@
         <v/>
       </c>
       <c r="I43" s="131">
-        <f>SUM(C43:H43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44327,7 +44329,7 @@
         <v/>
       </c>
       <c r="I44" s="131">
-        <f>SUM(C44:H44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44425,7 +44427,7 @@
         <v/>
       </c>
       <c r="I45" s="131">
-        <f>SUM(C45:H45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44523,7 +44525,7 @@
         <v/>
       </c>
       <c r="I46" s="131">
-        <f>SUM(C46:H46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44621,7 +44623,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="131">
-        <f>SUM(C47:H47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44719,7 +44721,7 @@
         <v/>
       </c>
       <c r="I48" s="131">
-        <f>SUM(C48:H48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44817,7 +44819,7 @@
         <v/>
       </c>
       <c r="I49" s="131">
-        <f>SUM(C49:H49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -44915,7 +44917,7 @@
         <v/>
       </c>
       <c r="I50" s="131">
-        <f>SUM(C50:H50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -45013,7 +45015,7 @@
         <v/>
       </c>
       <c r="I51" s="131">
-        <f>SUM(C51:H51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -45111,7 +45113,7 @@
         <v/>
       </c>
       <c r="I52" s="131">
-        <f>SUM(C52:H52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -45209,7 +45211,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="132">
-        <f>SUM(C53:H53)</f>
+        <f t="shared" si="1"/>
         <v>275</v>
       </c>
     </row>
@@ -45307,7 +45309,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="132">
-        <f>SUM(C54:H54)</f>
+        <f t="shared" si="1"/>
         <v>235</v>
       </c>
     </row>
@@ -45405,7 +45407,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="132">
-        <f>SUM(C55:H55)</f>
+        <f t="shared" si="1"/>
         <v>213</v>
       </c>
     </row>
@@ -45503,7 +45505,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="132">
-        <f>SUM(C56:H56)</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
     </row>
@@ -45601,7 +45603,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="132">
-        <f>SUM(C57:H57)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -45699,7 +45701,7 @@
         <v/>
       </c>
       <c r="I58" s="132">
-        <f>SUM(C58:H58)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -45797,7 +45799,7 @@
         <v/>
       </c>
       <c r="I59" s="132">
-        <f>SUM(C59:H59)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -45895,7 +45897,7 @@
         <v/>
       </c>
       <c r="I60" s="132">
-        <f>SUM(C60:H60)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -45993,7 +45995,7 @@
         <v/>
       </c>
       <c r="I61" s="132">
-        <f>SUM(C61:H61)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -46091,7 +46093,7 @@
         <v/>
       </c>
       <c r="I62" s="132">
-        <f>SUM(C62:H62)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -46189,7 +46191,7 @@
         <v/>
       </c>
       <c r="I63" s="132">
-        <f>SUM(C63:H63)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -46287,7 +46289,7 @@
         <v/>
       </c>
       <c r="I64" s="132">
-        <f>SUM(C64:H64)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -46385,7 +46387,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="133">
-        <f>SUM(C65:H65)</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
     </row>
@@ -46483,7 +46485,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="133">
-        <f>SUM(C66:H66)</f>
+        <f t="shared" ref="I66:I96" si="2">SUM(C66:H66)</f>
         <v>181</v>
       </c>
     </row>
@@ -46581,7 +46583,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="133">
-        <f>SUM(C67:H67)</f>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
     </row>
@@ -46679,7 +46681,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="133">
-        <f>SUM(C68:H68)</f>
+        <f t="shared" si="2"/>
         <v>162</v>
       </c>
     </row>
@@ -46777,7 +46779,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="133">
-        <f>SUM(C69:H69)</f>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
     </row>
@@ -46875,7 +46877,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="133">
-        <f>SUM(C70:H70)</f>
+        <f t="shared" si="2"/>
         <v>122</v>
       </c>
     </row>
@@ -46973,7 +46975,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="133">
-        <f>SUM(C71:H71)</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
     </row>
@@ -47071,7 +47073,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="133">
-        <f>SUM(C72:H72)</f>
+        <f t="shared" si="2"/>
         <v>101</v>
       </c>
     </row>
@@ -47169,7 +47171,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="133">
-        <f>SUM(C73:H73)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
     </row>
@@ -47267,7 +47269,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="133">
-        <f>SUM(C74:H74)</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
     </row>
@@ -47365,7 +47367,7 @@
         <v/>
       </c>
       <c r="I75" s="133">
-        <f>SUM(C75:H75)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -47463,7 +47465,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="133">
-        <f>SUM(C76:H76)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -47561,7 +47563,7 @@
         <v/>
       </c>
       <c r="I77" s="133">
-        <f>SUM(C77:H77)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -47659,7 +47661,7 @@
         <v/>
       </c>
       <c r="I78" s="133">
-        <f>SUM(C78:H78)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -47757,7 +47759,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="133">
-        <f>SUM(C79:H79)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -47855,7 +47857,7 @@
         <v/>
       </c>
       <c r="I80" s="133">
-        <f>SUM(C80:H80)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -47953,7 +47955,7 @@
         <v/>
       </c>
       <c r="I81" s="133">
-        <f>SUM(C81:H81)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -48051,7 +48053,7 @@
         <v/>
       </c>
       <c r="I82" s="133">
-        <f>SUM(C82:H82)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -48149,7 +48151,7 @@
         <v/>
       </c>
       <c r="I83" s="133">
-        <f>SUM(C83:H83)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -48247,7 +48249,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="134">
-        <f>SUM(C84:H84)</f>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
     </row>
@@ -48345,7 +48347,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="134">
-        <f>SUM(C85:H85)</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
     </row>
@@ -48443,7 +48445,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="134">
-        <f>SUM(C86:H86)</f>
+        <f t="shared" si="2"/>
         <v>189</v>
       </c>
     </row>
@@ -48541,7 +48543,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="134">
-        <f>SUM(C87:H87)</f>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
     </row>
@@ -48639,7 +48641,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="134">
-        <f>SUM(C88:H88)</f>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
     </row>
@@ -48737,7 +48739,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="134">
-        <f>SUM(C89:H89)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -48835,18 +48837,18 @@
         <v>0</v>
       </c>
       <c r="I90" s="134">
-        <f>SUM(C90:H90)</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A91" s="134" t="str">
-        <f>TeamHelper!I97</f>
+        <f>TeamHelper!I82</f>
         <v>Sr Boys</v>
       </c>
       <c r="B91" s="134" t="str">
-        <f>TeamHelper!H97</f>
-        <v>Whistler</v>
+        <f>TeamHelper!H82</f>
+        <v>Burnaby Mtn</v>
       </c>
       <c r="C91" s="134" cm="1">
         <f t="array" ref="C91">IFERROR(
@@ -48860,7 +48862,7 @@
   )),
   ""
 )</f>
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D91" s="134" cm="1">
         <f t="array" ref="D91">IFERROR(
@@ -48933,18 +48935,18 @@
         <v>0</v>
       </c>
       <c r="I91" s="134">
-        <f>SUM(C91:H91)</f>
-        <v>81</v>
+        <f t="shared" si="2"/>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A92" s="134" t="str">
-        <f>TeamHelper!I82</f>
+        <f>TeamHelper!I95</f>
         <v>Sr Boys</v>
       </c>
       <c r="B92" s="134" t="str">
-        <f>TeamHelper!H82</f>
-        <v>Burnaby Mtn</v>
+        <f>TeamHelper!H95</f>
+        <v>Sutherland</v>
       </c>
       <c r="C92" s="134" cm="1">
         <f t="array" ref="C92">IFERROR(
@@ -48958,7 +48960,7 @@
   )),
   ""
 )</f>
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="D92" s="134" cm="1">
         <f t="array" ref="D92">IFERROR(
@@ -49031,18 +49033,18 @@
         <v>0</v>
       </c>
       <c r="I92" s="134">
-        <f>SUM(C92:H92)</f>
-        <v>59</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A93" s="134" t="str">
-        <f>TeamHelper!I95</f>
+        <f>TeamHelper!I89</f>
         <v>Sr Boys</v>
       </c>
       <c r="B93" s="134" t="str">
-        <f>TeamHelper!H95</f>
-        <v>Sutherland</v>
+        <f>TeamHelper!H89</f>
+        <v>Mulgrave</v>
       </c>
       <c r="C93" s="134" cm="1">
         <f t="array" ref="C93">IFERROR(
@@ -49056,7 +49058,7 @@
   )),
   ""
 )</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D93" s="134" cm="1">
         <f t="array" ref="D93">IFERROR(
@@ -49129,18 +49131,18 @@
         <v>0</v>
       </c>
       <c r="I93" s="134">
-        <f>SUM(C93:H93)</f>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A94" s="134" t="str">
-        <f>TeamHelper!I89</f>
+        <f>TeamHelper!I81</f>
         <v>Sr Boys</v>
       </c>
       <c r="B94" s="134" t="str">
-        <f>TeamHelper!H89</f>
-        <v>Mulgrave</v>
+        <f>TeamHelper!H81</f>
+        <v>Brockton</v>
       </c>
       <c r="C94" s="134" cm="1">
         <f t="array" ref="C94">IFERROR(
@@ -49154,7 +49156,7 @@
   )),
   ""
 )</f>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D94" s="134" cm="1">
         <f t="array" ref="D94">IFERROR(
@@ -49227,20 +49229,20 @@
         <v>0</v>
       </c>
       <c r="I94" s="134">
-        <f>SUM(C94:H94)</f>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A95" s="134" t="str">
-        <f>TeamHelper!I81</f>
+        <f>TeamHelper!I84</f>
         <v>Sr Boys</v>
       </c>
       <c r="B95" s="134" t="str">
-        <f>TeamHelper!H81</f>
-        <v>Brockton</v>
-      </c>
-      <c r="C95" s="134" cm="1">
+        <f>TeamHelper!H84</f>
+        <v>Coast Mtn</v>
+      </c>
+      <c r="C95" s="134" t="str" cm="1">
         <f t="array" ref="C95">IFERROR(
   SUM(LARGE(
     IF(
@@ -49252,9 +49254,9 @@
   )),
   ""
 )</f>
-        <v>18</v>
-      </c>
-      <c r="D95" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="D95" s="134" t="str" cm="1">
         <f t="array" ref="D95">IFERROR(
   SUM(LARGE(
     IF(
@@ -49266,9 +49268,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="E95" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="E95" s="134" t="str" cm="1">
         <f t="array" ref="E95">IFERROR(
   SUM(LARGE(
     IF(
@@ -49280,9 +49282,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="F95" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="F95" s="134" t="str" cm="1">
         <f t="array" ref="F95">IFERROR(
   SUM(LARGE(
     IF(
@@ -49294,9 +49296,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="G95" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="G95" s="134" t="str" cm="1">
         <f t="array" ref="G95">IFERROR(
   SUM(LARGE(
     IF(
@@ -49308,9 +49310,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="H95" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="H95" s="134" t="str" cm="1">
         <f t="array" ref="H95">IFERROR(
   SUM(LARGE(
     IF(
@@ -49322,21 +49324,21 @@
   )),
   ""
 )</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I95" s="134">
-        <f>SUM(C95:H95)</f>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A96" s="134" t="str">
-        <f>TeamHelper!I84</f>
+        <f>TeamHelper!I85</f>
         <v>Sr Boys</v>
       </c>
       <c r="B96" s="134" t="str">
-        <f>TeamHelper!H84</f>
-        <v>Coast Mtn</v>
+        <f>TeamHelper!H85</f>
+        <v>Elphinstone</v>
       </c>
       <c r="C96" s="134" t="str" cm="1">
         <f t="array" ref="C96">IFERROR(
@@ -49423,20 +49425,20 @@
         <v/>
       </c>
       <c r="I96" s="134">
-        <f>SUM(C96:H96)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A97" s="134" t="str">
-        <f>TeamHelper!I85</f>
+        <f>TeamHelper!I86</f>
         <v>Sr Boys</v>
       </c>
       <c r="B97" s="134" t="str">
-        <f>TeamHelper!H85</f>
-        <v>Elphinstone</v>
-      </c>
-      <c r="C97" s="134" t="str" cm="1">
+        <f>TeamHelper!H86</f>
+        <v>GW Graham</v>
+      </c>
+      <c r="C97" s="134" cm="1">
         <f t="array" ref="C97">IFERROR(
   SUM(LARGE(
     IF(
@@ -49448,9 +49450,9 @@
   )),
   ""
 )</f>
-        <v/>
-      </c>
-      <c r="D97" s="134" t="str" cm="1">
+        <v>0</v>
+      </c>
+      <c r="D97" s="134" cm="1">
         <f t="array" ref="D97">IFERROR(
   SUM(LARGE(
     IF(
@@ -49462,9 +49464,9 @@
   )),
   ""
 )</f>
-        <v/>
-      </c>
-      <c r="E97" s="134" t="str" cm="1">
+        <v>0</v>
+      </c>
+      <c r="E97" s="134" cm="1">
         <f t="array" ref="E97">IFERROR(
   SUM(LARGE(
     IF(
@@ -49476,9 +49478,9 @@
   )),
   ""
 )</f>
-        <v/>
-      </c>
-      <c r="F97" s="134" t="str" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F97" s="134" cm="1">
         <f t="array" ref="F97">IFERROR(
   SUM(LARGE(
     IF(
@@ -49490,9 +49492,9 @@
   )),
   ""
 )</f>
-        <v/>
-      </c>
-      <c r="G97" s="134" t="str" cm="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="134" cm="1">
         <f t="array" ref="G97">IFERROR(
   SUM(LARGE(
     IF(
@@ -49504,9 +49506,9 @@
   )),
   ""
 )</f>
-        <v/>
-      </c>
-      <c r="H97" s="134" t="str" cm="1">
+        <v>0</v>
+      </c>
+      <c r="H97" s="134" cm="1">
         <f t="array" ref="H97">IFERROR(
   SUM(LARGE(
     IF(
@@ -49518,23 +49520,23 @@
   )),
   ""
 )</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I97" s="134">
-        <f>SUM(C97:H97)</f>
+        <f t="shared" ref="I97:I101" si="3">SUM(C97:H97)</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A98" s="134" t="str">
-        <f>TeamHelper!I86</f>
+        <f>TeamHelper!I91</f>
         <v>Sr Boys</v>
       </c>
       <c r="B98" s="134" t="str">
-        <f>TeamHelper!H86</f>
-        <v>GW Graham</v>
-      </c>
-      <c r="C98" s="134" cm="1">
+        <f>TeamHelper!H91</f>
+        <v>Rockridge</v>
+      </c>
+      <c r="C98" s="134" t="str" cm="1">
         <f t="array" ref="C98">IFERROR(
   SUM(LARGE(
     IF(
@@ -49546,9 +49548,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="D98" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="D98" s="134" t="str" cm="1">
         <f t="array" ref="D98">IFERROR(
   SUM(LARGE(
     IF(
@@ -49560,9 +49562,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="E98" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="E98" s="134" t="str" cm="1">
         <f t="array" ref="E98">IFERROR(
   SUM(LARGE(
     IF(
@@ -49574,9 +49576,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="F98" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="F98" s="134" t="str" cm="1">
         <f t="array" ref="F98">IFERROR(
   SUM(LARGE(
     IF(
@@ -49588,9 +49590,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="G98" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="G98" s="134" t="str" cm="1">
         <f t="array" ref="G98">IFERROR(
   SUM(LARGE(
     IF(
@@ -49602,9 +49604,9 @@
   )),
   ""
 )</f>
-        <v>0</v>
-      </c>
-      <c r="H98" s="134" cm="1">
+        <v/>
+      </c>
+      <c r="H98" s="134" t="str" cm="1">
         <f t="array" ref="H98">IFERROR(
   SUM(LARGE(
     IF(
@@ -49616,21 +49618,21 @@
   )),
   ""
 )</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I98" s="134">
-        <f>SUM(C98:H98)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A99" s="134" t="str">
-        <f>TeamHelper!I91</f>
+        <f>TeamHelper!I93</f>
         <v>Sr Boys</v>
       </c>
       <c r="B99" s="134" t="str">
-        <f>TeamHelper!H91</f>
-        <v>Rockridge</v>
+        <f>TeamHelper!H93</f>
+        <v>St. Georges</v>
       </c>
       <c r="C99" s="134" t="str" cm="1">
         <f t="array" ref="C99">IFERROR(
@@ -49717,18 +49719,18 @@
         <v/>
       </c>
       <c r="I99" s="134">
-        <f>SUM(C99:H99)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A100" s="134" t="str">
-        <f>TeamHelper!I93</f>
+        <f>TeamHelper!I94</f>
         <v>Sr Boys</v>
       </c>
       <c r="B100" s="134" t="str">
-        <f>TeamHelper!H93</f>
-        <v>St. Georges</v>
+        <f>TeamHelper!H94</f>
+        <v>STA</v>
       </c>
       <c r="C100" s="134" t="str" cm="1">
         <f t="array" ref="C100">IFERROR(
@@ -49815,18 +49817,18 @@
         <v/>
       </c>
       <c r="I100" s="134">
-        <f>SUM(C100:H100)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A101" s="134" t="str">
-        <f>TeamHelper!I94</f>
+        <f>TeamHelper!I96</f>
         <v>Sr Boys</v>
       </c>
       <c r="B101" s="134" t="str">
-        <f>TeamHelper!H94</f>
-        <v>STA</v>
+        <f>TeamHelper!H96</f>
+        <v>West Van</v>
       </c>
       <c r="C101" s="134" t="str" cm="1">
         <f t="array" ref="C101">IFERROR(
@@ -49913,210 +49915,14 @@
         <v/>
       </c>
       <c r="I101" s="134">
-        <f>SUM(C101:H101)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A102" s="134" t="str">
-        <f>TeamHelper!I96</f>
-        <v>Sr Boys</v>
-      </c>
-      <c r="B102" s="134" t="str">
-        <f>TeamHelper!H96</f>
-        <v>West Van</v>
-      </c>
-      <c r="C102" s="134" t="str" cm="1">
-        <f t="array" ref="C102">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A102) *
-      ('Individual Results'!$C$2:$C$411=$B102),
-      VALUE('Individual Results'!$G$2:$G$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="D102" s="134" t="str" cm="1">
-        <f t="array" ref="D102">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A102) *
-      ('Individual Results'!$C$2:$C$411=$B102),
-      VALUE('Individual Results'!$I$2:$I$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="E102" s="134" t="str" cm="1">
-        <f t="array" ref="E102">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A102) *
-      ('Individual Results'!$C$2:$C$411=$B102),
-      VALUE('Individual Results'!$K$2:$K$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="F102" s="134" t="str" cm="1">
-        <f t="array" ref="F102">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A102) *
-      ('Individual Results'!$C$2:$C$411=$B102),
-      VALUE('Individual Results'!$M$2:$M$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="G102" s="134" t="str" cm="1">
-        <f t="array" ref="G102">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A102) *
-      ('Individual Results'!$C$2:$C$411=$B102),
-      VALUE('Individual Results'!$O$2:$O$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="H102" s="134" t="str" cm="1">
-        <f t="array" ref="H102">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A102) *
-      ('Individual Results'!$C$2:$C$411=$B102),
-      VALUE('Individual Results'!$Q$2:$Q$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="I102" s="134">
-        <f>SUM(C102:H102)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A103" s="134" t="str">
-        <f>TeamHelper!I96</f>
-        <v>Sr Boys</v>
-      </c>
-      <c r="B103" s="134" t="str">
-        <f>TeamHelper!H96</f>
-        <v>West Van</v>
-      </c>
-      <c r="C103" s="134" t="str" cm="1">
-        <f t="array" ref="C103">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A103) *
-      ('Individual Results'!$C$2:$C$411=$B103),
-      VALUE('Individual Results'!$G$2:$G$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="D103" s="134" t="str" cm="1">
-        <f t="array" ref="D103">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A103) *
-      ('Individual Results'!$C$2:$C$411=$B103),
-      VALUE('Individual Results'!$I$2:$I$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="E103" s="134" t="str" cm="1">
-        <f t="array" ref="E103">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A103) *
-      ('Individual Results'!$C$2:$C$411=$B103),
-      VALUE('Individual Results'!$K$2:$K$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="F103" s="134" t="str" cm="1">
-        <f t="array" ref="F103">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A103) *
-      ('Individual Results'!$C$2:$C$411=$B103),
-      VALUE('Individual Results'!$M$2:$M$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="G103" s="134" t="str" cm="1">
-        <f t="array" ref="G103">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A103) *
-      ('Individual Results'!$C$2:$C$411=$B103),
-      VALUE('Individual Results'!$O$2:$O$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="H103" s="134" t="str" cm="1">
-        <f t="array" ref="H103">IFERROR(
-  SUM(LARGE(
-    IF(
-      ('Individual Results'!$D$2:$D$411=$A103) *
-      ('Individual Results'!$C$2:$C$411=$B103),
-      VALUE('Individual Results'!$Q$2:$Q$411)
-    ),
-    {1,2,3}
-  )),
-  ""
-)</f>
-        <v/>
-      </c>
-      <c r="I103" s="134">
-        <f>SUM(C103:H103)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I103">
-    <sortCondition ref="A2:A103"/>
-    <sortCondition descending="1" ref="I2:I103"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I101">
+    <sortCondition ref="A2:A101"/>
+    <sortCondition descending="1" ref="I2:I101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -50177,7 +49983,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="str" cm="1">
-        <f t="array" ref="A4:I22">_xlfn._xlws.FILTER(TeamPoints!A2:I108, TeamPoints!A2:A108 = B1)</f>
+        <f t="array" ref="A4:I22">_xlfn._xlws.FILTER(TeamPoints!A2:I106, TeamPoints!A2:A106 = B1)</f>
         <v>Juv Boys</v>
       </c>
       <c r="B4" s="19" t="str">

</xml_diff>